<commit_message>
Parte I + Introdução + Conclusão no relatório
</commit_message>
<xml_diff>
--- a/novos_inserts(se_precisarem).xlsx
+++ b/novos_inserts(se_precisarem).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ISEP\BDAD\Shared\bddad_tp1_2dl_g5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A95292D-9564-473E-8DE9-F8AF5C4F6768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941334C5-C962-434A-880F-F567B147CE7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{9C7D838C-1872-4758-893C-51B1FE701FD4}"/>
+    <workbookView xWindow="8970" yWindow="0" windowWidth="11520" windowHeight="10515" activeTab="1" xr2:uid="{9C7D838C-1872-4758-893C-51B1FE701FD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="100">
   <si>
     <t>Distritos</t>
   </si>
@@ -333,7 +333,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -370,9 +370,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,7 +691,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,10 +1926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F582B92-9215-4B5D-888B-5CFB8B15BA0C}">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,7 +2009,7 @@
         <v>96</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D61" si="0">A3-30</f>
+        <f t="shared" ref="D3:D66" si="0">A3-30</f>
         <v>44015</v>
       </c>
       <c r="E3">
@@ -2019,7 +2020,7 @@
         <v>100000002</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G61" si="1">_xlfn.CONCAT("INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('",TEXT(A3,"AAAA-MM-DD"),"', '",TEXT(B3,"AAAA-MM-DD"),"', '",C3,"', '",TEXT(D3,"AAAA-MM-DD"),"', ",E3,", ",F3,");")</f>
+        <f t="shared" ref="G3:G66" si="1">_xlfn.CONCAT("INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('",TEXT(A3,"AAAA-MM-DD"),"', '",TEXT(B3,"AAAA-MM-DD"),"', '",C3,"', '",TEXT(D3,"AAAA-MM-DD"),"', ",E3,", ",F3,");")</f>
         <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-08-02', '2020-08-14', 'single', '2020-07-03', 1, 100000002);</v>
       </c>
       <c r="L3" t="s">
@@ -3212,11 +3213,11 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <f t="shared" ref="A47:A50" si="4">A46+1</f>
+        <f t="shared" ref="A47:A49" si="4">A46+1</f>
         <v>43833</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" ref="B47:B50" si="5">B46+1</f>
+        <f t="shared" ref="B47:B49" si="5">B46+1</f>
         <v>43835</v>
       </c>
       <c r="C47" t="s">
@@ -3605,6 +3606,284 @@
       <c r="G61" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-10-06', '2020-10-15', 'suite', '2020-09-06', 4, 100000004);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B62" s="2">
+        <v>43953</v>
+      </c>
+      <c r="C62" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="0"/>
+        <v>43922</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <f>Clientes!B6</f>
+        <v>100000005</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-05-01', '2020-05-02', 'single', '2020-04-01', 1, 100000005);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <f>A62+1</f>
+        <v>43953</v>
+      </c>
+      <c r="B63" s="2">
+        <f>B62+1</f>
+        <v>43954</v>
+      </c>
+      <c r="C63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="0"/>
+        <v>43923</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <f>Clientes!B7</f>
+        <v>100000006</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-05-02', '2020-05-03', 'twin', '2020-04-02', 2, 100000006);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <f t="shared" ref="A64:A65" si="8">A63+1</f>
+        <v>43954</v>
+      </c>
+      <c r="B64" s="2">
+        <f t="shared" ref="B64:B65" si="9">B63+1</f>
+        <v>43955</v>
+      </c>
+      <c r="C64" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="0"/>
+        <v>43924</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <f>Clientes!B8</f>
+        <v>100000007</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-05-03', '2020-05-04', 'suite', '2020-04-03', 3, 100000007);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <f t="shared" si="8"/>
+        <v>43955</v>
+      </c>
+      <c r="B65" s="2">
+        <f t="shared" si="9"/>
+        <v>43956</v>
+      </c>
+      <c r="C65" t="s">
+        <v>99</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="0"/>
+        <v>43925</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <f>Clientes!B9</f>
+        <v>100000008</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-05-04', '2020-05-05', 'suite', '2020-04-04', 3, 100000008);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <f>A65+1</f>
+        <v>43956</v>
+      </c>
+      <c r="B66" s="2">
+        <f>B65+1</f>
+        <v>43957</v>
+      </c>
+      <c r="C66" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="0"/>
+        <v>43926</v>
+      </c>
+      <c r="E66">
+        <v>4</v>
+      </c>
+      <c r="F66">
+        <f>Clientes!B10</f>
+        <v>100000009</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-05-05', '2020-05-06', 'superior', '2020-04-05', 4, 100000009);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <f>A62+61</f>
+        <v>44013</v>
+      </c>
+      <c r="B67" s="2">
+        <f>B62+61</f>
+        <v>44014</v>
+      </c>
+      <c r="C67" t="s">
+        <v>98</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D71" si="10">A67-30</f>
+        <v>43983</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="F67">
+        <f>Clientes!B11</f>
+        <v>100000010</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" ref="G67:G71" si="11">_xlfn.CONCAT("INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('",TEXT(A67,"AAAA-MM-DD"),"', '",TEXT(B67,"AAAA-MM-DD"),"', '",C67,"', '",TEXT(D67,"AAAA-MM-DD"),"', ",E67,", ",F67,");")</f>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-07-01', '2020-07-02', 'superior', '2020-06-01', 4, 100000010);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <f>A67+1</f>
+        <v>44014</v>
+      </c>
+      <c r="B68" s="2">
+        <f>B67+1</f>
+        <v>44015</v>
+      </c>
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="10"/>
+        <v>43984</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <f>Clientes!B12</f>
+        <v>100000011</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-07-02', '2020-07-03', 'suite', '2020-06-02', 3, 100000011);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <f t="shared" ref="A69:A71" si="12">A68+1</f>
+        <v>44015</v>
+      </c>
+      <c r="B69" s="2">
+        <f t="shared" ref="B69:B71" si="13">B68+1</f>
+        <v>44016</v>
+      </c>
+      <c r="C69" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="10"/>
+        <v>43985</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <f>Clientes!B13</f>
+        <v>100000012</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-07-03', '2020-07-04', 'suite', '2020-06-03', 3, 100000012);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <f t="shared" si="12"/>
+        <v>44016</v>
+      </c>
+      <c r="B70" s="2">
+        <f t="shared" si="13"/>
+        <v>44017</v>
+      </c>
+      <c r="C70" t="s">
+        <v>95</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="10"/>
+        <v>43986</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <f>Clientes!B14</f>
+        <v>100000013</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-07-04', '2020-07-05', 'twin', '2020-06-04', 2, 100000013);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <f t="shared" si="12"/>
+        <v>44017</v>
+      </c>
+      <c r="B71" s="2">
+        <f t="shared" si="13"/>
+        <v>44018</v>
+      </c>
+      <c r="C71" t="s">
+        <v>96</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="10"/>
+        <v>43987</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <f>Clientes!B15</f>
+        <v>100000014</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO reserva (dataEntrada, dataSaida, tipoQuarto, dataReserva, numeroPessoas, clienteNIF) VALUES('2020-07-05', '2020-07-06', 'single', '2020-06-05', 1, 100000014);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>